<commit_message>
Fix 3-Year Summary category alignment in infrastructure-costs.xlsx files
Fixed 9 files with misaligned categories between Infrastructure Costs,
Credits, and 3-Year Summary sheets:

- Azure DevOps Enterprise Platform
- Dell VxRail HCI, VxRail Hyperconverged, SafeID, PowerEdge CI, PowerSwitch
- GitHub Advanced Security, Actions Enterprise CI/CD
- Google Modern Workspace

Issues fixed:
- Removed orphan "savings" rows that had no corresponding source data
- Added missing categories from Credits sheet to 3-Year Summary
- Rebuilt SUMIF formulas to reference correct category names
- Cleared stray data below TOTAL rows

All 35 files now have properly aligned categories for accurate cost rollups.
</commit_message>
<xml_diff>
--- a/solutions/azure/devops/enterprise-platform/presales/infrastructure-costs.xlsx
+++ b/solutions/azure/devops/enterprise-platform/presales/infrastructure-costs.xlsx
@@ -1968,7 +1968,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -2095,7 +2095,7 @@
     <row r="5" ht="26" customHeight="1">
       <c r="A5" s="43" t="inlineStr">
         <is>
-          <t>Support &amp; Maintenance</t>
+          <t>Hardware</t>
         </is>
       </c>
       <c r="B5" s="46">
@@ -2126,34 +2126,97 @@
     <row r="6" ht="26" customHeight="1">
       <c r="A6" s="51" t="inlineStr">
         <is>
+          <t>Support &amp; Maintenance</t>
+        </is>
+      </c>
+      <c r="B6" s="53">
+        <f>SUMIF('Infrastructure Costs'!$A:$A,A6,'Infrastructure Costs'!$G:$G)</f>
+        <v/>
+      </c>
+      <c r="C6" s="53">
+        <f>SUMIF(Credits!$A:$A,A6,Credits!$C:$C)</f>
+        <v/>
+      </c>
+      <c r="D6" s="53">
+        <f>B6+C6</f>
+        <v/>
+      </c>
+      <c r="E6" s="53">
+        <f>SUMIF('Infrastructure Costs'!$A:$A,A6,'Infrastructure Costs'!$H:$H)</f>
+        <v/>
+      </c>
+      <c r="F6" s="53">
+        <f>SUMIF('Infrastructure Costs'!$A:$A,A6,'Infrastructure Costs'!$I:$I)</f>
+        <v/>
+      </c>
+      <c r="G6" s="53">
+        <f>D6+E6+F6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Professional Services</t>
+        </is>
+      </c>
+      <c r="B7">
+        <f>SUMIF('Infrastructure Costs'!$A:$A,A7,'Infrastructure Costs'!$G:$G)</f>
+        <v/>
+      </c>
+      <c r="C7">
+        <f>SUMIF(Credits!$A:$A,A7,Credits!$C:$C)</f>
+        <v/>
+      </c>
+      <c r="D7">
+        <f>B7+C7</f>
+        <v/>
+      </c>
+      <c r="E7">
+        <f>SUMIF('Infrastructure Costs'!$A:$A,A7,'Infrastructure Costs'!$H:$H)</f>
+        <v/>
+      </c>
+      <c r="F7">
+        <f>SUMIF('Infrastructure Costs'!$A:$A,A7,'Infrastructure Costs'!$I:$I)</f>
+        <v/>
+      </c>
+      <c r="G7">
+        <f>D7+E7+F7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B6" s="53">
-        <f>SUM(B3:B5)</f>
-        <v/>
-      </c>
-      <c r="C6" s="53">
-        <f>SUM(C3:C5)</f>
-        <v/>
-      </c>
-      <c r="D6" s="53">
-        <f>SUM(D3:D5)</f>
-        <v/>
-      </c>
-      <c r="E6" s="53">
-        <f>SUM(E3:E5)</f>
-        <v/>
-      </c>
-      <c r="F6" s="53">
-        <f>SUM(F3:F5)</f>
-        <v/>
-      </c>
-      <c r="G6" s="53">
-        <f>SUM(G3:G5)</f>
-        <v/>
-      </c>
-    </row>
+      <c r="B8">
+        <f>SUM(B3:B7)</f>
+        <v/>
+      </c>
+      <c r="C8">
+        <f>SUM(C3:C7)</f>
+        <v/>
+      </c>
+      <c r="D8">
+        <f>SUM(D3:D7)</f>
+        <v/>
+      </c>
+      <c r="E8">
+        <f>SUM(E3:E7)</f>
+        <v/>
+      </c>
+      <c r="F8">
+        <f>SUM(F3:F7)</f>
+        <v/>
+      </c>
+      <c r="G8">
+        <f>SUM(G3:G7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9"/>
   </sheetData>
   <autoFilter ref="A2:G6"/>
   <mergeCells count="1">

</xml_diff>